<commit_message>
Homepage for users (student login). display student courses and information (wip).
</commit_message>
<xml_diff>
--- a/ManagementSystem/src/main/java/com/example/phase1_1420/UMS_Data.xlsx
+++ b/ManagementSystem/src/main/java/com/example/phase1_1420/UMS_Data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="185">
   <si>
     <t>Subject Code</t>
   </si>
@@ -584,9 +584,6 @@
   </si>
   <si>
     <t>Electron22</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
 </sst>
 </file>

</xml_diff>